<commit_message>
almost done, uml and scrum completed and a vew error checks
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" tabRatio="627"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" tabRatio="627" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="193">
   <si>
     <t>Product Name:</t>
   </si>
@@ -493,6 +493,126 @@
   </si>
   <si>
     <t>* Get familiar/installing with fltk</t>
+  </si>
+  <si>
+    <t>None were made due to studying for a test</t>
+  </si>
+  <si>
+    <t>No Progress was due here</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Start to be able to build windows</t>
+  </si>
+  <si>
+    <t>Start to be able to build Buttons</t>
+  </si>
+  <si>
+    <t>Undersetanding of callBacks</t>
+  </si>
+  <si>
+    <t>Open window in gui</t>
+  </si>
+  <si>
+    <t>task 2</t>
+  </si>
+  <si>
+    <t>task 3</t>
+  </si>
+  <si>
+    <t>task 4</t>
+  </si>
+  <si>
+    <t>Create Robot Parts</t>
+  </si>
+  <si>
+    <t>Used pointer callbacks</t>
+  </si>
+  <si>
+    <t>Create Robot Models</t>
+  </si>
+  <si>
+    <t>Display Models List</t>
+  </si>
+  <si>
+    <t>Loop through parts for models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store and post models </t>
+  </si>
+  <si>
+    <t xml:space="preserve">task 5 </t>
+  </si>
+  <si>
+    <t>task 6</t>
+  </si>
+  <si>
+    <t>task 7</t>
+  </si>
+  <si>
+    <t>task 8</t>
+  </si>
+  <si>
+    <t>task 9</t>
+  </si>
+  <si>
+    <t>task 10</t>
+  </si>
+  <si>
+    <t>task 11</t>
+  </si>
+  <si>
+    <t>task 12</t>
+  </si>
+  <si>
+    <t>create customer</t>
+  </si>
+  <si>
+    <t>create sales</t>
+  </si>
+  <si>
+    <t>create order</t>
+  </si>
+  <si>
+    <t>load to csv files</t>
+  </si>
+  <si>
+    <t>save to csv files</t>
+  </si>
+  <si>
+    <t>load and save to specific files</t>
+  </si>
+  <si>
+    <t>copy and past from multi output</t>
+  </si>
+  <si>
+    <t>view all orders</t>
+  </si>
+  <si>
+    <t>Before making order ask for customer info</t>
+  </si>
+  <si>
+    <t>Create employees</t>
+  </si>
+  <si>
+    <t>Create order and view it</t>
+  </si>
+  <si>
+    <t>save to files for no loosing of history</t>
+  </si>
+  <si>
+    <t>load from files into vectors</t>
+  </si>
+  <si>
+    <t>load from and save to specific files</t>
+  </si>
+  <si>
+    <t>copy and paste to fill in part numbers</t>
+  </si>
+  <si>
+    <t>save to order files, laod and display</t>
   </si>
 </sst>
 </file>
@@ -602,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,6 +796,7 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +904,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -834,31 +954,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>36.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,11 +994,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1184183216"/>
-        <c:axId val="1184186944"/>
+        <c:axId val="74552064"/>
+        <c:axId val="196270576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1184183216"/>
+        <c:axId val="74552064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +1022,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -915,7 +1034,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1184186944"/>
+        <c:crossAx val="196270576"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -923,7 +1042,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1184186944"/>
+        <c:axId val="196270576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +1075,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -970,7 +1088,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1184183216"/>
+        <c:crossAx val="74552064"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1086,28 +1204,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,11 +1241,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1184215280"/>
-        <c:axId val="1184219040"/>
+        <c:axId val="151650288"/>
+        <c:axId val="156854992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1184215280"/>
+        <c:axId val="151650288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1164,7 +1282,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1184219040"/>
+        <c:crossAx val="156854992"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1172,7 +1290,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1184219040"/>
+        <c:axId val="156854992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1337,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1184215280"/>
+        <c:crossAx val="151650288"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1335,28 +1453,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,11 +1490,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1184246464"/>
-        <c:axId val="1184250224"/>
+        <c:axId val="157166848"/>
+        <c:axId val="157169968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1184246464"/>
+        <c:axId val="157166848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1531,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1184250224"/>
+        <c:crossAx val="157169968"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1539,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1184250224"/>
+        <c:axId val="157169968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1586,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1184246464"/>
+        <c:crossAx val="157166848"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1538,7 +1656,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.151063900396577"/>
+          <c:y val="0.0853080568720379"/>
+          <c:w val="0.834887193924678"/>
+          <c:h val="0.817290741500914"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="1"/>
@@ -1584,28 +1712,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1621,11 +1749,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1147533536"/>
-        <c:axId val="1147536656"/>
+        <c:axId val="156969664"/>
+        <c:axId val="157022176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1147533536"/>
+        <c:axId val="156969664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1662,7 +1790,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1147536656"/>
+        <c:crossAx val="157022176"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1670,7 +1798,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1147536656"/>
+        <c:axId val="157022176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,7 +1831,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00351222641968617"/>
+              <c:y val="0.42401238944658"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1717,7 +1852,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1147533536"/>
+        <c:crossAx val="156969664"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1833,28 +1968,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1870,11 +2005,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1147569872"/>
-        <c:axId val="1147573632"/>
+        <c:axId val="72028896"/>
+        <c:axId val="157000320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1147569872"/>
+        <c:axId val="72028896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,7 +2046,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1147573632"/>
+        <c:crossAx val="157000320"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1919,7 +2054,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1147573632"/>
+        <c:axId val="157000320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1966,7 +2101,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1147569872"/>
+        <c:crossAx val="72028896"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2075,28 +2210,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2112,11 +2247,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1105743856"/>
-        <c:axId val="1105747616"/>
+        <c:axId val="151384608"/>
+        <c:axId val="151387728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1105743856"/>
+        <c:axId val="151384608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,7 +2288,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1105747616"/>
+        <c:crossAx val="151387728"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2161,7 +2296,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1105747616"/>
+        <c:axId val="151387728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2343,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1105743856"/>
+        <c:crossAx val="151384608"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2783,12 +2918,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="1"/>
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
@@ -3041,8 +3177,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="6">
-        <f>COUNT(B34:B149)</f>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>7</v>
@@ -3060,8 +3195,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" ref="B22:B29" si="0">B21</f>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>10</v>
@@ -3079,14 +3213,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="8">
-        <f t="shared" ref="D23:D28" si="1">D22+7</f>
+        <f t="shared" ref="D23:D28" si="0">D22+7</f>
         <v>42656</v>
       </c>
       <c r="E23" s="3"/>
@@ -3099,14 +3232,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42663</v>
       </c>
       <c r="E24" s="3"/>
@@ -3119,14 +3251,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42670</v>
       </c>
       <c r="E25" s="3"/>
@@ -3138,15 +3269,14 @@
       <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="B26" s="32">
+        <v>16</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42677</v>
       </c>
       <c r="E26" s="3"/>
@@ -3158,15 +3288,14 @@
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="B27" s="32">
+        <v>15</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42684</v>
       </c>
       <c r="E27" s="3"/>
@@ -3178,15 +3307,14 @@
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="B28" s="32">
+        <v>12</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42691</v>
       </c>
       <c r="E28" s="3"/>
@@ -3198,9 +3326,8 @@
       <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="B29" s="32">
+        <v>0</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>14</v>
@@ -3276,10 +3403,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="78" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B34">
         <v>1</v>
       </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
       <c r="E34" s="1">
         <v>1</v>
       </c>
@@ -3296,10 +3426,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B35" s="13">
         <v>2</v>
       </c>
+      <c r="D35" s="13">
+        <v>2</v>
+      </c>
       <c r="E35" s="14">
         <v>1</v>
       </c>
@@ -3316,10 +3449,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="208" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="B36">
         <v>3</v>
       </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
       <c r="E36" s="1">
         <v>1</v>
       </c>
@@ -3336,10 +3472,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="13" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B37" s="13">
         <v>4</v>
       </c>
+      <c r="D37" s="13">
+        <v>2</v>
+      </c>
       <c r="E37" s="14">
         <v>1</v>
       </c>
@@ -3356,10 +3495,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="91" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B38">
         <v>5</v>
       </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
       <c r="E38" s="1">
         <v>1</v>
       </c>
@@ -3376,10 +3518,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="13" customFormat="1" ht="91" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" s="13" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B39" s="13">
         <v>6</v>
       </c>
+      <c r="D39" s="13">
+        <v>3</v>
+      </c>
       <c r="E39" s="14">
         <v>1</v>
       </c>
@@ -3396,10 +3541,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="169" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B40">
         <v>7</v>
       </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
       <c r="E40" s="1">
         <v>1</v>
       </c>
@@ -3416,7 +3564,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="143" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B41">
         <v>8</v>
       </c>
@@ -3436,10 +3584,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="13" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" s="13" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B42" s="13">
         <v>9</v>
       </c>
+      <c r="D42" s="13">
+        <v>3</v>
+      </c>
       <c r="E42" s="14">
         <v>1</v>
       </c>
@@ -3456,10 +3607,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="130" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B43">
         <v>10</v>
       </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
@@ -3476,10 +3630,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="117" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B44">
         <v>11</v>
       </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
       <c r="E44" s="1">
         <v>1</v>
       </c>
@@ -3496,10 +3653,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="65" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B45">
         <v>12</v>
       </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
       <c r="E45" s="1">
         <v>1</v>
       </c>
@@ -3514,7 +3674,7 @@
       </c>
       <c r="I45" s="12"/>
     </row>
-    <row r="46" spans="1:9" s="16" customFormat="1" ht="130" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" s="16" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B46">
         <v>13</v>
       </c>
@@ -3534,10 +3694,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="16" customFormat="1" ht="143" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" s="16" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B47">
         <v>14</v>
       </c>
+      <c r="D47" s="16">
+        <v>8</v>
+      </c>
       <c r="E47" s="17">
         <v>2</v>
       </c>
@@ -3554,10 +3717,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="16" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" s="16" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B48">
         <v>15</v>
       </c>
+      <c r="D48" s="16">
+        <v>8</v>
+      </c>
       <c r="E48" s="17">
         <v>2</v>
       </c>
@@ -3574,10 +3740,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="2:9" s="16" customFormat="1" ht="156" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:9" s="16" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B49">
         <v>16</v>
       </c>
+      <c r="D49" s="16">
+        <v>8</v>
+      </c>
       <c r="E49" s="17">
         <v>2</v>
       </c>
@@ -3594,7 +3763,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="2:9" s="19" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:9" s="19" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B50" s="16">
         <v>23</v>
       </c>
@@ -3614,7 +3783,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="2:9" s="19" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:9" s="19" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B51" s="16">
         <v>24</v>
       </c>
@@ -3634,7 +3803,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="2:9" s="25" customFormat="1" ht="273" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:9" s="25" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="B52" s="25">
         <v>17</v>
       </c>
@@ -3654,10 +3823,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="25" customFormat="1" ht="156" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:9" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B53" s="25">
         <v>18</v>
       </c>
+      <c r="D53" s="25">
+        <v>8</v>
+      </c>
       <c r="E53" s="26">
         <v>3</v>
       </c>
@@ -3677,7 +3849,7 @@
     <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="E54"/>
     </row>
-    <row r="56" spans="2:9" s="25" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:9" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B56">
         <v>21</v>
       </c>
@@ -3697,7 +3869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="2:9" s="25" customFormat="1" ht="169" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:9" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B57">
         <v>22</v>
       </c>
@@ -3717,7 +3889,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="2:9" s="25" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:9" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B58" s="25">
         <v>25</v>
       </c>
@@ -3737,10 +3909,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="2:9" s="25" customFormat="1" ht="182" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:9" s="25" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="B59" s="25">
         <v>26</v>
       </c>
+      <c r="D59" s="25">
+        <v>8</v>
+      </c>
       <c r="E59" s="26">
         <v>3</v>
       </c>
@@ -3757,7 +3932,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="2:9" s="28" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:9" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B60" s="28">
         <v>27</v>
       </c>
@@ -3777,7 +3952,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="2:9" s="28" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:9" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B61" s="28">
         <v>28</v>
       </c>
@@ -3797,7 +3972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="2:9" s="28" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:9" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B62" s="28">
         <v>19</v>
       </c>
@@ -3817,7 +3992,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="2:9" s="28" customFormat="1" ht="91" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B63" s="28">
         <v>20</v>
       </c>
@@ -3837,7 +4012,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="2:9" s="28" customFormat="1" ht="156" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:9" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B64" s="28">
         <v>29</v>
       </c>
@@ -3857,7 +4032,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="2:9" s="28" customFormat="1" ht="143" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:9" s="28" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B65" s="28">
         <v>30</v>
       </c>
@@ -3877,7 +4052,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="130" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B66">
         <v>31</v>
       </c>
@@ -3897,7 +4072,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="130" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B67">
         <v>32</v>
       </c>
@@ -3917,7 +4092,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="130" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B68">
         <v>33</v>
       </c>
@@ -3937,7 +4112,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="130" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B69">
         <v>34</v>
       </c>
@@ -3957,7 +4132,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="78" x14ac:dyDescent="0.15">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B70">
         <v>35</v>
       </c>
@@ -3977,7 +4152,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="156" x14ac:dyDescent="0.15">
+    <row r="71" spans="2:9" ht="26" x14ac:dyDescent="0.15">
       <c r="B71">
         <v>36</v>
       </c>
@@ -4009,15 +4184,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -4089,7 +4265,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="32">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -4104,7 +4280,7 @@
       </c>
       <c r="B7" s="32">
         <f t="shared" ref="B7:B13" si="0">B6</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -4119,7 +4295,7 @@
       </c>
       <c r="B8" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
@@ -4134,7 +4310,7 @@
       </c>
       <c r="B9" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -4149,7 +4325,7 @@
       </c>
       <c r="B10" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
@@ -4164,7 +4340,7 @@
       </c>
       <c r="B11" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -4179,7 +4355,7 @@
       </c>
       <c r="B12" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -4194,7 +4370,7 @@
       </c>
       <c r="B13" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
@@ -4237,6 +4413,11 @@
       </c>
       <c r="H15" s="10" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F16" s="33" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4251,16 +4432,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -4332,7 +4513,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="32">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -4347,7 +4528,7 @@
       </c>
       <c r="B7" s="32">
         <f t="shared" ref="B7:B13" si="0">B6</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -4362,7 +4543,7 @@
       </c>
       <c r="B8" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
@@ -4377,7 +4558,7 @@
       </c>
       <c r="B9" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -4392,7 +4573,7 @@
       </c>
       <c r="B10" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
@@ -4407,7 +4588,7 @@
       </c>
       <c r="B11" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -4422,7 +4603,7 @@
       </c>
       <c r="B12" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -4437,7 +4618,7 @@
       </c>
       <c r="B13" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
@@ -4489,8 +4670,13 @@
       <c r="B16" t="s">
         <v>151</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="33" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F17" s="33" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4505,19 +4691,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="32">
+        <v>3</v>
+      </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
@@ -4529,7 +4722,9 @@
       <c r="A2" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="31">
+        <v>42677.333333333336</v>
+      </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
@@ -4541,7 +4736,9 @@
       <c r="A3" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="31">
+        <v>42684.333333333336</v>
+      </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -4576,7 +4773,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="32">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -4591,7 +4788,7 @@
       </c>
       <c r="B7" s="32">
         <f t="shared" ref="B7:B13" si="0">B6</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -4606,7 +4803,7 @@
       </c>
       <c r="B8" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
@@ -4621,7 +4818,7 @@
       </c>
       <c r="B9" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -4636,7 +4833,7 @@
       </c>
       <c r="B10" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
@@ -4650,8 +4847,7 @@
         <v>139</v>
       </c>
       <c r="B11" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -4665,8 +4861,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -4681,7 +4876,7 @@
       </c>
       <c r="B13" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
@@ -4724,6 +4919,27 @@
       </c>
       <c r="H15" s="10" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F18" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4738,19 +4954,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" activeCellId="1" sqref="F1 G16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="32">
+        <v>4</v>
+      </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
@@ -4762,7 +4986,9 @@
       <c r="A2" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="31">
+        <v>42684.333333333336</v>
+      </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
@@ -4774,7 +5000,9 @@
       <c r="A3" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="31">
+        <v>42691.333333333336</v>
+      </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -4809,7 +5037,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="32">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -4823,8 +5051,7 @@
         <v>135</v>
       </c>
       <c r="B7" s="32">
-        <f t="shared" ref="B7:B13" si="0">B6</f>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -4838,8 +5065,7 @@
         <v>136</v>
       </c>
       <c r="B8" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
@@ -4853,8 +5079,8 @@
         <v>137</v>
       </c>
       <c r="B9" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f t="shared" ref="B9:B10" si="0">B8</f>
+        <v>11</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -4869,7 +5095,7 @@
       </c>
       <c r="B10" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
@@ -4883,8 +5109,7 @@
         <v>139</v>
       </c>
       <c r="B11" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -4898,8 +5123,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -4913,8 +5137,7 @@
         <v>141</v>
       </c>
       <c r="B13" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
@@ -4957,6 +5180,39 @@
       </c>
       <c r="H15" s="10" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -4971,19 +5227,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2">
+        <v>5</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -4995,7 +5258,9 @@
       <c r="A2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="31">
+        <v>42691.333333333336</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5007,7 +5272,9 @@
       <c r="A3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="31">
+        <v>42696.333333333336</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -5042,7 +5309,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="32">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -5056,8 +5323,8 @@
         <v>135</v>
       </c>
       <c r="B7" s="32">
-        <f t="shared" ref="B7:B13" si="0">B6</f>
-        <v>23</v>
+        <f t="shared" ref="B7:B9" si="0">B6</f>
+        <v>8</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -5072,7 +5339,7 @@
       </c>
       <c r="B8" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -5087,7 +5354,7 @@
       </c>
       <c r="B9" s="32">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -5101,8 +5368,7 @@
         <v>138</v>
       </c>
       <c r="B10" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -5116,8 +5382,7 @@
         <v>139</v>
       </c>
       <c r="B11" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -5131,8 +5396,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -5146,8 +5410,7 @@
         <v>141</v>
       </c>
       <c r="B13" s="32">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -5192,6 +5455,94 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" t="s">
+        <v>183</v>
+      </c>
+      <c r="F22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>

</xml_diff>